<commit_message>
refine images and UI
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinyoung/Google 드라이브/1. 2018시즌 전반기/1. HCI개론/CS374_Team_Accel_Excel_PoKaChip/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remin\WebstormProjects\2018_CS374\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7A707DD1-F3F3-6F41-AFA9-0FA2420AED1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{FCC991B3-B0D9-574F-BF8B-293DFAF82F48}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GPU" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>모델명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -264,16 +263,32 @@
   </si>
   <si>
     <t>보드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>펜티엄 G4560</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.5(3.5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://prod.danawa.com/info/?pcode=4827935</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
-    <numFmt numFmtId="176" formatCode="&quot;₩&quot;#,##0"/>
+    <numFmt numFmtId="176" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
+    <numFmt numFmtId="177" formatCode="&quot;₩&quot;#,##0"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -343,10 +358,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -357,7 +372,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="기본" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -669,27 +684,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0233AC9-2F5B-7D49-BA69-90AE93E7ACA8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView zoomScale="182" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" customWidth="1"/>
-    <col min="10" max="10" width="66.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="38.44140625" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" customWidth="1"/>
+    <col min="10" max="10" width="66.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="72">
+    <row r="1" spans="1:10" ht="69">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1017,9 +1032,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J8" r:id="rId1" xr:uid="{054B5F7A-1083-EE4A-AA1C-4B7BA68B2F7B}"/>
-    <hyperlink ref="J2" r:id="rId2" xr:uid="{F9F0510F-F792-424E-B763-4B3655DA5A9F}"/>
-    <hyperlink ref="J3" r:id="rId3" xr:uid="{051D7923-C88C-9A46-9F44-D02FAB740970}"/>
+    <hyperlink ref="J8" r:id="rId1"/>
+    <hyperlink ref="J2" r:id="rId2"/>
+    <hyperlink ref="J3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1027,23 +1042,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16505557-4090-0541-834F-641358638EAD}">
-  <dimension ref="A1:M8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" style="6" customWidth="1"/>
-    <col min="13" max="13" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="41.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="54">
+    <row r="1" spans="1:13" ht="51.75">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1089,43 +1104,43 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="C2" s="4">
-        <v>61220</v>
+        <v>47470</v>
       </c>
       <c r="D2" s="4">
-        <v>106790</v>
+        <v>71400</v>
       </c>
       <c r="E2" s="4">
-        <f>SUM(C2:D2)</f>
-        <v>168010</v>
+        <f>SUM(D2,C2)</f>
+        <v>118870</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="5">
-        <v>570</v>
-      </c>
-      <c r="I2" s="5">
-        <v>146</v>
+        <v>63</v>
+      </c>
+      <c r="H2" s="6">
+        <v>369</v>
+      </c>
+      <c r="I2" s="6">
+        <v>147</v>
       </c>
       <c r="J2" s="5">
-        <f>H2/$H$2*50+I2/$I$2*50</f>
-        <v>100</v>
+        <f>H2/$H$3*50+I2/$I$3*50</f>
+        <v>82.710886806056237</v>
       </c>
       <c r="K2" s="6">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="L2" s="6">
-        <f>K2/$K$2*100</f>
-        <v>100</v>
+        <f>K2/$K$3*100</f>
+        <v>71.929824561403507</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1133,43 +1148,43 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="4">
-        <v>82780</v>
+        <v>61220</v>
       </c>
       <c r="D3" s="4">
-        <v>128260</v>
+        <v>106790</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E8" si="0">SUM(C3:D3)</f>
-        <v>211040</v>
+        <f>SUM(C3:D3)</f>
+        <v>168010</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" s="5">
-        <v>611</v>
+        <v>570</v>
       </c>
       <c r="I3" s="5">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3:J8" si="1">H3/$H$2*50+I3/$I$2*50</f>
-        <v>112.15813506368661</v>
+        <f>H3/$H$3*50+I3/$I$3*50</f>
+        <v>100</v>
       </c>
       <c r="K3" s="6">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L3" s="6">
-        <f t="shared" ref="L3:L8" si="2">K3/$K$2*100</f>
-        <v>105.26315789473684</v>
+        <f>K3/$K$3*100</f>
+        <v>100</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1177,43 +1192,43 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="4">
-        <v>61220</v>
+        <v>82780</v>
       </c>
       <c r="D4" s="4">
-        <v>181790</v>
+        <v>128260</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" si="0"/>
-        <v>243010</v>
+        <f t="shared" ref="E4:E9" si="0">SUM(C4:D4)</f>
+        <v>211040</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H4" s="5">
-        <v>810</v>
+        <v>611</v>
       </c>
       <c r="I4" s="5">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="J4" s="5">
-        <f t="shared" si="1"/>
-        <v>123.10742609949531</v>
+        <f t="shared" ref="J4:J9" si="1">H4/$H$3*50+I4/$I$3*50</f>
+        <v>112.15813506368661</v>
       </c>
       <c r="K4" s="6">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L4" s="6">
-        <f t="shared" si="2"/>
-        <v>107.01754385964912</v>
+        <f t="shared" ref="L4:L9" si="2">K4/$K$3*100</f>
+        <v>105.26315789473684</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1221,43 +1236,43 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="4">
-        <v>82780</v>
+        <v>61220</v>
       </c>
       <c r="D5" s="4">
-        <v>225780</v>
+        <v>181790</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>308560</v>
+        <v>243010</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H5" s="5">
-        <v>981</v>
+        <v>810</v>
       </c>
       <c r="I5" s="5">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="1"/>
-        <v>144.27180966113914</v>
+        <v>123.10742609949531</v>
       </c>
       <c r="K5" s="6">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" si="2"/>
-        <v>115.78947368421053</v>
+        <v>107.01754385964912</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1265,43 +1280,43 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="4">
-        <v>61220</v>
+        <v>82780</v>
       </c>
       <c r="D6" s="4">
-        <v>245000</v>
+        <v>225780</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>306220</v>
+        <v>308560</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H6" s="5">
-        <v>1284</v>
+        <v>981</v>
       </c>
       <c r="I6" s="5">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="1"/>
-        <v>170.50829127613554</v>
+        <v>144.27180966113914</v>
       </c>
       <c r="K6" s="6">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" si="2"/>
-        <v>110.5263157894737</v>
+        <v>115.78947368421053</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1309,43 +1324,43 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="4">
-        <v>82780</v>
+        <v>61220</v>
       </c>
       <c r="D7" s="4">
-        <v>251150</v>
+        <v>245000</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>333930</v>
+        <v>306220</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H7" s="5">
-        <v>1051</v>
+        <v>1284</v>
       </c>
       <c r="I7" s="5">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="1"/>
-        <v>154.52174957942802</v>
+        <v>170.50829127613554</v>
       </c>
       <c r="K7" s="6">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L7" s="6">
         <f t="shared" si="2"/>
-        <v>117.54385964912282</v>
+        <v>110.5263157894737</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1353,57 +1368,102 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="4">
-        <v>61220</v>
+        <v>82780</v>
       </c>
       <c r="D8" s="4">
-        <v>284000</v>
+        <v>251150</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>345220</v>
+        <v>333930</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H8" s="5">
-        <v>1379</v>
+        <v>1051</v>
       </c>
       <c r="I8" s="5">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="1"/>
-        <v>180.55395337659218</v>
+        <v>154.52174957942802</v>
       </c>
       <c r="K8" s="6">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" si="2"/>
+        <v>117.54385964912282</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4">
+        <v>61220</v>
+      </c>
+      <c r="D9" s="4">
+        <v>284000</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>345220</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1379</v>
+      </c>
+      <c r="I9" s="5">
+        <v>174</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="1"/>
+        <v>180.55395337659218</v>
+      </c>
+      <c r="K9" s="6">
+        <v>65</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" si="2"/>
         <v>114.03508771929825</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1" xr:uid="{7F61C66E-DE80-A946-92B2-1460CFFAA31B}"/>
-    <hyperlink ref="M6" r:id="rId2" xr:uid="{240C8E9D-EBE0-7D41-91CA-4C44B9E9075B}"/>
-    <hyperlink ref="M4" r:id="rId3" xr:uid="{22CC2761-45B6-934C-A9A3-AA38D75D4FDA}"/>
-    <hyperlink ref="M2" r:id="rId4" xr:uid="{73B326FD-09F7-1D49-8775-02AF94E87160}"/>
-    <hyperlink ref="M5" r:id="rId5" xr:uid="{1FBA5492-5F60-5842-BD78-DBB72EB80C51}"/>
-    <hyperlink ref="M7" r:id="rId6" xr:uid="{03DEA927-DABE-EA4D-BB6C-120092468717}"/>
-    <hyperlink ref="M8" r:id="rId7" xr:uid="{B5A9202B-FEAC-9C43-BDC2-E586E356DDB8}"/>
+    <hyperlink ref="M4" r:id="rId1"/>
+    <hyperlink ref="M7" r:id="rId2"/>
+    <hyperlink ref="M5" r:id="rId3"/>
+    <hyperlink ref="M3" r:id="rId4"/>
+    <hyperlink ref="M6" r:id="rId5"/>
+    <hyperlink ref="M8" r:id="rId6"/>
+    <hyperlink ref="M9" r:id="rId7"/>
+    <hyperlink ref="M2" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Set DB, minor fix
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remin\WebstormProjects\2018_CS374\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reminiel\WebstormProjects\2018_CS374\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1045,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="E8" sqref="E7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25"/>
@@ -1129,8 +1129,8 @@
         <v>147</v>
       </c>
       <c r="J2" s="5">
-        <f>H2/$H$3*50+I2/$I$3*50</f>
-        <v>82.710886806056237</v>
+        <f>H2/$H$3*30+I2/$I$3*70</f>
+        <v>89.900504686373466</v>
       </c>
       <c r="K2" s="6">
         <v>41</v>
@@ -1173,7 +1173,7 @@
         <v>146</v>
       </c>
       <c r="J3" s="5">
-        <f>H3/$H$3*50+I3/$I$3*50</f>
+        <f t="shared" ref="J3:J9" si="0">H3/$H$3*30+I3/$I$3*70</f>
         <v>100</v>
       </c>
       <c r="K3" s="6">
@@ -1201,7 +1201,7 @@
         <v>128260</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E9" si="0">SUM(C4:D4)</f>
+        <f t="shared" ref="E4:E9" si="1">SUM(C4:D4)</f>
         <v>211040</v>
       </c>
       <c r="F4" t="s">
@@ -1217,8 +1217,8 @@
         <v>171</v>
       </c>
       <c r="J4" s="5">
-        <f t="shared" ref="J4:J9" si="1">H4/$H$3*50+I4/$I$3*50</f>
-        <v>112.15813506368661</v>
+        <f t="shared" si="0"/>
+        <v>114.14419610670512</v>
       </c>
       <c r="K4" s="6">
         <v>60</v>
@@ -1245,7 +1245,7 @@
         <v>181790</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>243010</v>
       </c>
       <c r="F5" t="s">
@@ -1261,8 +1261,8 @@
         <v>152</v>
       </c>
       <c r="J5" s="5">
-        <f t="shared" si="1"/>
-        <v>123.10742609949531</v>
+        <f t="shared" si="0"/>
+        <v>115.50829127613554</v>
       </c>
       <c r="K5" s="6">
         <v>61</v>
@@ -1289,7 +1289,7 @@
         <v>225780</v>
       </c>
       <c r="E6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>308560</v>
       </c>
       <c r="F6" t="s">
@@ -1305,8 +1305,8 @@
         <v>170</v>
       </c>
       <c r="J6" s="5">
-        <f t="shared" si="1"/>
-        <v>144.27180966113914</v>
+        <f t="shared" si="0"/>
+        <v>133.13842826243692</v>
       </c>
       <c r="K6" s="6">
         <v>66</v>
@@ -1333,7 +1333,7 @@
         <v>245000</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>306220</v>
       </c>
       <c r="F7" t="s">
@@ -1349,8 +1349,8 @@
         <v>169</v>
       </c>
       <c r="J7" s="5">
-        <f t="shared" si="1"/>
-        <v>170.50829127613554</v>
+        <f t="shared" si="0"/>
+        <v>148.60634462869501</v>
       </c>
       <c r="K7" s="6">
         <v>63</v>
@@ -1377,7 +1377,7 @@
         <v>251150</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>333930</v>
       </c>
       <c r="F8" t="s">
@@ -1393,8 +1393,8 @@
         <v>182</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" si="1"/>
-        <v>154.52174957942802</v>
+        <f t="shared" si="0"/>
+        <v>142.57606344628695</v>
       </c>
       <c r="K8" s="6">
         <v>67</v>
@@ -1421,7 +1421,7 @@
         <v>284000</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>345220</v>
       </c>
       <c r="F9" t="s">
@@ -1437,8 +1437,8 @@
         <v>174</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" si="1"/>
-        <v>180.55395337659218</v>
+        <f t="shared" si="0"/>
+        <v>156.00360490266763</v>
       </c>
       <c r="K9" s="6">
         <v>65</v>

</xml_diff>

<commit_message>
Add & fix multiple issues
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -75,198 +75,202 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>리드텍 GTX1060 6GB WinFast HURRICANE OC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://prod.danawa.com/info/?pcode=5540425</t>
+  </si>
+  <si>
+    <t>http://prod.danawa.com/info/?pcode=5078717</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://prod.danawa.com/info/?pcode=5540416</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>표준 점수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baffle Ground 상옵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baffle Ground 풀옵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클럭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>라이젠 3 2200G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i3 8100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>라이젠 5 2400G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i5 8500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>라이젠 5 2600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i5 8600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>라이젠 5 2600X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코어(쓰레드)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU값</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>총액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://prod.danawa.com/info/?pcode=5530456</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6(6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.1(4.3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.0(4.1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6(12)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.6(4.25)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.4(3.9)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://prod.danawa.com/info/?pcode=6066396</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://prod.danawa.com/info/?pcode=5884096</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4(8)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.6(3.9)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://prod.danawa.com/info/?pcode=5884539</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.5(3.7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.6(3.6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://prod.danawa.com/info/?pcode=6020667</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://prod.danawa.com/info/?pcode=6020678</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://prod.danawa.com/info/?pcode=6066419</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>표준 점수(Cinebench R15 Multi)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>표준 점수 백분율</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baffle Ground 풀옵(최저 프레임)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baffle Ground 풀옵(백분율)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>표준 점수(Cinebench R15 Single)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>펜티엄 G4560</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inno3D GTX1060 3GB X2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가상 지표</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>http://prod.danawa.com/info/?pcode=4360032</t>
-  </si>
-  <si>
-    <t>리드텍 GTX1060 6GB WinFast HURRICANE OC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://prod.danawa.com/info/?pcode=5540425</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>http://prod.danawa.com/info/?pcode=4796979</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>http://prod.danawa.com/info/?pcode=4260047</t>
-  </si>
-  <si>
-    <t>http://prod.danawa.com/info/?pcode=5078717</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>http://prod.danawa.com/info/?pcode=5089139</t>
-  </si>
-  <si>
-    <t>Code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://prod.danawa.com/info/?pcode=5540416</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>표준 점수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Baffle Ground 상옵</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Baffle Ground 풀옵</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>클럭</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>라이젠 3 2200G</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>i3 8100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>라이젠 5 2400G</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>i5 8500</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>라이젠 5 2600</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>i5 8600</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>라이젠 5 2600X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>코어(쓰레드)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CPU값</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>총액</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4(4)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://prod.danawa.com/info/?pcode=5530456</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6(6)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.1(4.3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.0(4.1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6(12)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.6(4.25)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.4(3.9)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://prod.danawa.com/info/?pcode=6066396</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://prod.danawa.com/info/?pcode=5884096</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4(8)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.6(3.9)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://prod.danawa.com/info/?pcode=5884539</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.5(3.7)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.6(3.6)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://prod.danawa.com/info/?pcode=6020667</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://prod.danawa.com/info/?pcode=6020678</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://prod.danawa.com/info/?pcode=6066419</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>표준 점수(Cinebench R15 Multi)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>표준 점수 백분율</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Baffle Ground 풀옵(최저 프레임)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Baffle Ground 풀옵(백분율)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>표준 점수(Cinebench R15 Single)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>보드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>펜티엄 G4560</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>inno3D GTX1060 3GB X2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가상 지표</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -676,7 +680,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView zoomScale="182" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25"/>
@@ -694,7 +698,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="69">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -712,13 +716,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -729,7 +733,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -763,7 +767,7 @@
         <v>39</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -795,8 +799,8 @@
       <c r="I4">
         <v>45</v>
       </c>
-      <c r="J4" t="s">
-        <v>12</v>
+      <c r="J4" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -804,7 +808,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3">
         <v>398790</v>
@@ -828,7 +832,7 @@
         <v>49</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -860,8 +864,8 @@
       <c r="I6">
         <v>50</v>
       </c>
-      <c r="J6" t="s">
-        <v>15</v>
+      <c r="J6" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="17.100000000000001" customHeight="1">
@@ -893,8 +897,8 @@
       <c r="I7">
         <v>51</v>
       </c>
-      <c r="J7" t="s">
-        <v>16</v>
+      <c r="J7" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -927,7 +931,7 @@
         <v>53</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -955,8 +959,8 @@
       <c r="I9">
         <v>54</v>
       </c>
-      <c r="J9" t="s">
-        <v>18</v>
+      <c r="J9" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="10:10">
@@ -1000,9 +1004,13 @@
   <hyperlinks>
     <hyperlink ref="J8" r:id="rId1"/>
     <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="J4" r:id="rId3"/>
+    <hyperlink ref="J6" r:id="rId4"/>
+    <hyperlink ref="J7" r:id="rId5"/>
+    <hyperlink ref="J9" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1010,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="175" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25"/>
@@ -1025,43 +1033,43 @@
   <sheetData>
     <row r="1" spans="1:14" ht="51.75">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="K1" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="N1" t="s">
         <v>5</v>
@@ -1072,7 +1080,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="C2">
+        <v>51660</v>
+      </c>
+      <c r="D2">
+        <f>E2-C2</f>
+        <v>68100</v>
+      </c>
+      <c r="E2">
+        <v>119760</v>
       </c>
       <c r="H2" s="6">
         <v>369</v>
@@ -1091,7 +1109,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4">
         <v>61220</v>
@@ -1104,10 +1122,10 @@
         <v>168010</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H3" s="5">
         <v>570</v>
@@ -1131,7 +1149,7 @@
         <v>100</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1139,7 +1157,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4">
         <v>82780</v>
@@ -1152,10 +1170,10 @@
         <v>211040</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H4" s="5">
         <v>611</v>
@@ -1179,7 +1197,7 @@
         <v>105.26315789473684</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1187,7 +1205,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4">
         <v>61220</v>
@@ -1200,10 +1218,10 @@
         <v>243010</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H5" s="5">
         <v>810</v>
@@ -1227,7 +1245,7 @@
         <v>107.01754385964912</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1235,7 +1253,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C6" s="4">
         <v>82780</v>
@@ -1248,10 +1266,10 @@
         <v>308560</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H6" s="5">
         <v>981</v>
@@ -1275,7 +1293,7 @@
         <v>115.78947368421053</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1283,7 +1301,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C7" s="4">
         <v>61220</v>
@@ -1296,10 +1314,10 @@
         <v>306220</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H7" s="5">
         <v>1284</v>
@@ -1323,7 +1341,7 @@
         <v>110.5263157894737</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1331,7 +1349,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C8" s="4">
         <v>82780</v>
@@ -1344,10 +1362,10 @@
         <v>333930</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H8" s="5">
         <v>1051</v>
@@ -1371,7 +1389,7 @@
         <v>117.54385964912282</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1379,7 +1397,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C9" s="4">
         <v>61220</v>
@@ -1392,10 +1410,10 @@
         <v>345220</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H9" s="5">
         <v>1379</v>
@@ -1419,7 +1437,7 @@
         <v>114.03508771929825</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:14">

</xml_diff>